<commit_message>
Done with first elimination pass.  Need to finish second elimination pass.
</commit_message>
<xml_diff>
--- a/Bruce_CTT_data.xlsx
+++ b/Bruce_CTT_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brucemallory/MSSP/755 Measurement &amp; Psychometrics Theory/Assgn_1(CTT)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4134F9C0-373A-C448-B09A-24434222E7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7095FBEE-369C-8E4D-9EEB-C393A128741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="5520" windowWidth="21600" windowHeight="15700" activeTab="2" xr2:uid="{D2FCA387-96D5-3541-B4B2-260415E7B913}"/>
+    <workbookView xWindow="-21600" yWindow="5520" windowWidth="21600" windowHeight="15700" xr2:uid="{D2FCA387-96D5-3541-B4B2-260415E7B913}"/>
   </bookViews>
   <sheets>
     <sheet name="Responses" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="150">
   <si>
     <t>Education should empower people to be their best</t>
   </si>
@@ -484,6 +484,9 @@
   <si>
     <t>Score</t>
   </si>
+  <si>
+    <t>cutoff: change to find item scores higher than x</t>
+  </si>
 </sst>
 </file>
 
@@ -589,7 +592,94 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -945,13 +1035,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0306057C-2408-A84E-8BC5-C7D6D6F6716B}">
-  <dimension ref="A1:CN31"/>
+  <dimension ref="A1:CN33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="17" topLeftCell="CK18" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="17" topLeftCell="CJ18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7908,10 +7998,23 @@
         <v>140</v>
       </c>
     </row>
+    <row r="33" spans="89:90" x14ac:dyDescent="0.2">
+      <c r="CK33" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="CL33" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:D24">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CK2:CK24">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>$CK$33</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7923,7 +8026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B84AA0-4981-A640-B6F7-93E85735DCAD}">
   <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="Y2" sqref="Y2:Y83"/>
     </sheetView>
   </sheetViews>
@@ -14113,7 +14216,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:W83 Y1">
-    <cfRule type="containsBlanks" dxfId="3" priority="2">
+    <cfRule type="containsBlanks" dxfId="12" priority="2">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14125,7 +14228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5960A252-6C8C-3B49-8C8C-09DF97E5D8DF}">
   <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+    <sheetView topLeftCell="E25" workbookViewId="0">
       <selection activeCell="P58" sqref="P58"/>
     </sheetView>
   </sheetViews>
@@ -20950,7 +21053,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:W83">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="11" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ready for second culling pass
</commit_message>
<xml_diff>
--- a/Bruce_CTT_data.xlsx
+++ b/Bruce_CTT_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brucemallory/MSSP/755 Measurement &amp; Psychometrics Theory/Assgn_1(CTT)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7095FBEE-369C-8E4D-9EEB-C393A128741D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9384ACB5-D6E8-C54D-82B7-1EC2796DC300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="5520" windowWidth="21600" windowHeight="15700" xr2:uid="{D2FCA387-96D5-3541-B4B2-260415E7B913}"/>
+    <workbookView xWindow="-21600" yWindow="11440" windowWidth="21600" windowHeight="15700" activeTab="1" xr2:uid="{D2FCA387-96D5-3541-B4B2-260415E7B913}"/>
   </bookViews>
   <sheets>
     <sheet name="Responses" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="149">
   <si>
     <t>Education should empower people to be their best</t>
   </si>
@@ -482,9 +482,6 @@
     <t>NOTE: score/items and mean of means are not eaqual because of the few blanks in the data.</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
     <t>cutoff: change to find item scores higher than x</t>
   </si>
 </sst>
@@ -592,11 +589,24 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="4">
     <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -617,106 +627,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1037,7 +947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0306057C-2408-A84E-8BC5-C7D6D6F6716B}">
   <dimension ref="A1:CN33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="5" ySplit="17" topLeftCell="CJ18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
@@ -8003,7 +7913,7 @@
         <v>3.3</v>
       </c>
       <c r="CL33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -8026,8 +7936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B84AA0-4981-A640-B6F7-93E85735DCAD}">
   <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:Y83"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8106,9 +8016,7 @@
       <c r="W1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Y1" s="15" t="s">
-        <v>148</v>
-      </c>
+      <c r="Y1" s="15"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -8180,10 +8088,6 @@
       <c r="W2">
         <v>2</v>
       </c>
-      <c r="Y2" s="3">
-        <f>SUM(A2:W2)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -8255,10 +8159,6 @@
       <c r="W3">
         <v>2</v>
       </c>
-      <c r="Y3" s="3">
-        <f t="shared" ref="Y3:Y66" si="0">SUM(A3:W3)</f>
-        <v>60</v>
-      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -8330,10 +8230,6 @@
       <c r="W4">
         <v>3</v>
       </c>
-      <c r="Y4" s="3">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -8405,10 +8301,6 @@
       <c r="W5">
         <v>3</v>
       </c>
-      <c r="Y5" s="3">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -8474,10 +8366,6 @@
       <c r="V6">
         <v>2</v>
       </c>
-      <c r="Y6" s="3">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -8549,10 +8437,6 @@
       <c r="W7">
         <v>2</v>
       </c>
-      <c r="Y7" s="3">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -8624,10 +8508,6 @@
       <c r="W8">
         <v>3</v>
       </c>
-      <c r="Y8" s="3">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -8699,10 +8579,6 @@
       <c r="W9">
         <v>3</v>
       </c>
-      <c r="Y9" s="3">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -8765,10 +8641,6 @@
       <c r="W10">
         <v>3</v>
       </c>
-      <c r="Y10" s="3">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -8840,10 +8712,6 @@
       <c r="W11">
         <v>2</v>
       </c>
-      <c r="Y11" s="3">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -8915,10 +8783,6 @@
       <c r="W12">
         <v>3</v>
       </c>
-      <c r="Y12" s="3">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -8990,10 +8854,6 @@
       <c r="W13">
         <v>2</v>
       </c>
-      <c r="Y13" s="3">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -9065,10 +8925,6 @@
       <c r="W14">
         <v>2</v>
       </c>
-      <c r="Y14" s="3">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -9140,10 +8996,6 @@
       <c r="W15">
         <v>3</v>
       </c>
-      <c r="Y15" s="3">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -9206,12 +9058,8 @@
       <c r="W16">
         <v>2</v>
       </c>
-      <c r="Y16" s="3">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
@@ -9281,12 +9129,8 @@
       <c r="W17">
         <v>1</v>
       </c>
-      <c r="Y17" s="3">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4</v>
       </c>
@@ -9356,12 +9200,8 @@
       <c r="W18">
         <v>4</v>
       </c>
-      <c r="Y18" s="3">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -9431,12 +9271,8 @@
       <c r="W19">
         <v>2</v>
       </c>
-      <c r="Y19" s="3">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4</v>
       </c>
@@ -9506,12 +9342,8 @@
       <c r="W20">
         <v>3</v>
       </c>
-      <c r="Y20" s="3">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -9581,12 +9413,8 @@
       <c r="W21">
         <v>3</v>
       </c>
-      <c r="Y21" s="3">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -9656,12 +9484,8 @@
       <c r="W22">
         <v>3</v>
       </c>
-      <c r="Y22" s="3">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4</v>
       </c>
@@ -9731,12 +9555,8 @@
       <c r="W23">
         <v>3</v>
       </c>
-      <c r="Y23" s="3">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
@@ -9806,12 +9626,8 @@
       <c r="W24">
         <v>3</v>
       </c>
-      <c r="Y24" s="3">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -9881,12 +9697,8 @@
       <c r="W25">
         <v>3</v>
       </c>
-      <c r="Y25" s="3">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3</v>
       </c>
@@ -9956,12 +9768,8 @@
       <c r="W26">
         <v>4</v>
       </c>
-      <c r="Y26" s="3">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3</v>
       </c>
@@ -10031,12 +9839,8 @@
       <c r="W27">
         <v>3</v>
       </c>
-      <c r="Y27" s="3">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -10106,12 +9910,8 @@
       <c r="W28">
         <v>3</v>
       </c>
-      <c r="Y28" s="3">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -10181,12 +9981,8 @@
       <c r="W29">
         <v>3</v>
       </c>
-      <c r="Y29" s="3">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -10256,12 +10052,8 @@
       <c r="W30">
         <v>3</v>
       </c>
-      <c r="Y30" s="3">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -10331,12 +10123,8 @@
       <c r="W31">
         <v>2</v>
       </c>
-      <c r="Y31" s="3">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -10406,12 +10194,8 @@
       <c r="W32">
         <v>4</v>
       </c>
-      <c r="Y32" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -10478,12 +10262,8 @@
       <c r="W33">
         <v>2</v>
       </c>
-      <c r="Y33" s="3">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -10553,12 +10333,8 @@
       <c r="W34">
         <v>4</v>
       </c>
-      <c r="Y34" s="3">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3</v>
       </c>
@@ -10628,12 +10404,8 @@
       <c r="W35">
         <v>3</v>
       </c>
-      <c r="Y35" s="3">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -10703,12 +10475,8 @@
       <c r="W36">
         <v>4</v>
       </c>
-      <c r="Y36" s="3">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>4</v>
       </c>
@@ -10778,12 +10546,8 @@
       <c r="W37">
         <v>3</v>
       </c>
-      <c r="Y37" s="3">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>4</v>
       </c>
@@ -10853,12 +10617,8 @@
       <c r="W38">
         <v>2</v>
       </c>
-      <c r="Y38" s="3">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>4</v>
       </c>
@@ -10928,12 +10688,8 @@
       <c r="W39">
         <v>3</v>
       </c>
-      <c r="Y39" s="3">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>4</v>
       </c>
@@ -11003,12 +10759,8 @@
       <c r="W40">
         <v>3</v>
       </c>
-      <c r="Y40" s="3">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>4</v>
       </c>
@@ -11078,12 +10830,8 @@
       <c r="W41">
         <v>1</v>
       </c>
-      <c r="Y41" s="3">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>4</v>
       </c>
@@ -11153,12 +10901,8 @@
       <c r="W42">
         <v>3</v>
       </c>
-      <c r="Y42" s="3">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3</v>
       </c>
@@ -11228,12 +10972,8 @@
       <c r="W43">
         <v>2</v>
       </c>
-      <c r="Y43" s="3">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>4</v>
       </c>
@@ -11303,12 +11043,8 @@
       <c r="W44">
         <v>4</v>
       </c>
-      <c r="Y44" s="3">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>4</v>
       </c>
@@ -11378,12 +11114,8 @@
       <c r="W45">
         <v>1</v>
       </c>
-      <c r="Y45" s="3">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>4</v>
       </c>
@@ -11453,12 +11185,8 @@
       <c r="W46">
         <v>3</v>
       </c>
-      <c r="Y46" s="3">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3</v>
       </c>
@@ -11525,12 +11253,8 @@
       <c r="W47">
         <v>3</v>
       </c>
-      <c r="Y47" s="3">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>4</v>
       </c>
@@ -11600,12 +11324,8 @@
       <c r="W48">
         <v>3</v>
       </c>
-      <c r="Y48" s="3">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -11675,12 +11395,8 @@
       <c r="W49">
         <v>2</v>
       </c>
-      <c r="Y49" s="3">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>4</v>
       </c>
@@ -11750,12 +11466,8 @@
       <c r="W50" s="1">
         <v>3</v>
       </c>
-      <c r="Y50" s="3">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3</v>
       </c>
@@ -11823,12 +11535,8 @@
       <c r="W51" s="1">
         <v>2</v>
       </c>
-      <c r="Y51" s="3">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>4</v>
       </c>
@@ -11898,12 +11606,8 @@
       <c r="W52" s="1">
         <v>3</v>
       </c>
-      <c r="Y52" s="3">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3</v>
       </c>
@@ -11973,12 +11677,8 @@
       <c r="W53" s="1">
         <v>3</v>
       </c>
-      <c r="Y53" s="3">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>4</v>
       </c>
@@ -12048,12 +11748,8 @@
       <c r="W54" s="1">
         <v>3</v>
       </c>
-      <c r="Y54" s="3">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>4</v>
       </c>
@@ -12123,12 +11819,8 @@
       <c r="W55" s="1">
         <v>4</v>
       </c>
-      <c r="Y55" s="3">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>4</v>
       </c>
@@ -12198,12 +11890,8 @@
       <c r="W56" s="1">
         <v>3</v>
       </c>
-      <c r="Y56" s="3">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>4</v>
       </c>
@@ -12273,12 +11961,8 @@
       <c r="W57" s="1">
         <v>3</v>
       </c>
-      <c r="Y57" s="3">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>3</v>
       </c>
@@ -12346,12 +12030,8 @@
         <v>4</v>
       </c>
       <c r="W58" s="1"/>
-      <c r="Y58" s="3">
-        <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>4</v>
       </c>
@@ -12421,12 +12101,8 @@
       <c r="W59" s="1">
         <v>4</v>
       </c>
-      <c r="Y59" s="3">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>4</v>
       </c>
@@ -12496,12 +12172,8 @@
       <c r="W60" s="1">
         <v>4</v>
       </c>
-      <c r="Y60" s="3">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>3</v>
       </c>
@@ -12569,12 +12241,8 @@
         <v>3</v>
       </c>
       <c r="W61" s="1"/>
-      <c r="Y61" s="3">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>3</v>
       </c>
@@ -12644,12 +12312,8 @@
       <c r="W62" s="1">
         <v>2</v>
       </c>
-      <c r="Y62" s="3">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>3</v>
       </c>
@@ -12719,12 +12383,8 @@
       <c r="W63" s="1">
         <v>3</v>
       </c>
-      <c r="Y63" s="3">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>4</v>
       </c>
@@ -12794,12 +12454,8 @@
       <c r="W64" s="1">
         <v>3</v>
       </c>
-      <c r="Y64" s="3">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>4</v>
       </c>
@@ -12869,12 +12525,8 @@
       <c r="W65" s="1">
         <v>4</v>
       </c>
-      <c r="Y65" s="3">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>4</v>
       </c>
@@ -12944,12 +12596,8 @@
       <c r="W66" s="1">
         <v>3</v>
       </c>
-      <c r="Y66" s="3">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>4</v>
       </c>
@@ -13019,12 +12667,8 @@
       <c r="W67" s="1">
         <v>1</v>
       </c>
-      <c r="Y67" s="3">
-        <f t="shared" ref="Y67:Y83" si="1">SUM(A67:W67)</f>
-        <v>51</v>
-      </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>4</v>
       </c>
@@ -13094,12 +12738,8 @@
       <c r="W68" s="1">
         <v>1</v>
       </c>
-      <c r="Y68" s="3">
-        <f t="shared" si="1"/>
-        <v>49</v>
-      </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>4</v>
       </c>
@@ -13169,12 +12809,8 @@
       <c r="W69" s="1">
         <v>3</v>
       </c>
-      <c r="Y69" s="3">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>4</v>
       </c>
@@ -13234,12 +12870,8 @@
       <c r="W70" s="1">
         <v>3</v>
       </c>
-      <c r="Y70" s="3">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>3</v>
       </c>
@@ -13309,12 +12941,8 @@
       <c r="W71" s="1">
         <v>3</v>
       </c>
-      <c r="Y71" s="3">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>4</v>
       </c>
@@ -13384,12 +13012,8 @@
       <c r="W72" s="1">
         <v>3</v>
       </c>
-      <c r="Y72" s="3">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>3</v>
       </c>
@@ -13459,12 +13083,8 @@
       <c r="W73" s="1">
         <v>2</v>
       </c>
-      <c r="Y73" s="3">
-        <f t="shared" si="1"/>
-        <v>58</v>
-      </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>4</v>
       </c>
@@ -13534,12 +13154,8 @@
       <c r="W74" s="1">
         <v>2</v>
       </c>
-      <c r="Y74" s="3">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>4</v>
       </c>
@@ -13609,12 +13225,8 @@
       <c r="W75" s="1">
         <v>2</v>
       </c>
-      <c r="Y75" s="3">
-        <f t="shared" si="1"/>
-        <v>57</v>
-      </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>4</v>
       </c>
@@ -13684,12 +13296,8 @@
       <c r="W76" s="1">
         <v>3</v>
       </c>
-      <c r="Y76" s="3">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>4</v>
       </c>
@@ -13759,12 +13367,8 @@
       <c r="W77" s="1">
         <v>4</v>
       </c>
-      <c r="Y77" s="3">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>4</v>
       </c>
@@ -13834,12 +13438,8 @@
       <c r="W78" s="1">
         <v>3</v>
       </c>
-      <c r="Y78" s="3">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>4</v>
       </c>
@@ -13909,12 +13509,8 @@
       <c r="W79" s="1">
         <v>2</v>
       </c>
-      <c r="Y79" s="3">
-        <f t="shared" si="1"/>
-        <v>53</v>
-      </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>3</v>
       </c>
@@ -13984,12 +13580,8 @@
       <c r="W80" s="1">
         <v>3</v>
       </c>
-      <c r="Y80" s="3">
-        <f t="shared" si="1"/>
-        <v>61</v>
-      </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>4</v>
       </c>
@@ -14059,12 +13651,8 @@
       <c r="W81" s="1">
         <v>2</v>
       </c>
-      <c r="Y81" s="3">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>3</v>
       </c>
@@ -14134,12 +13722,8 @@
       <c r="W82" s="1">
         <v>3</v>
       </c>
-      <c r="Y82" s="3">
-        <f t="shared" si="1"/>
-        <v>62</v>
-      </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>3</v>
       </c>
@@ -14208,15 +13792,11 @@
       </c>
       <c r="W83" s="1">
         <v>3</v>
-      </c>
-      <c r="Y83" s="3">
-        <f t="shared" si="1"/>
-        <v>64</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:W83 Y1">
-    <cfRule type="containsBlanks" dxfId="12" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21053,7 +20633,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:W83">
-    <cfRule type="containsBlanks" dxfId="11" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
done and handed in
</commit_message>
<xml_diff>
--- a/Bruce_CTT_data.xlsx
+++ b/Bruce_CTT_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brucemallory/MSSP/755 Measurement &amp; Psychometrics Theory/Assgn_1(CTT)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9384ACB5-D6E8-C54D-82B7-1EC2796DC300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6142C6FA-03FC-964D-BD9E-8819629617B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="11440" windowWidth="21600" windowHeight="15700" activeTab="1" xr2:uid="{D2FCA387-96D5-3541-B4B2-260415E7B913}"/>
+    <workbookView xWindow="-21600" yWindow="11440" windowWidth="21600" windowHeight="15700" xr2:uid="{D2FCA387-96D5-3541-B4B2-260415E7B913}"/>
   </bookViews>
   <sheets>
     <sheet name="Responses" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="147">
   <si>
     <t>Education should empower people to be their best</t>
   </si>
@@ -470,12 +470,6 @@
     <t>KEEP?</t>
   </si>
   <si>
-    <t>NOTE: psych::alpha() marked Q3, 4, 11 and 15 as negatively correlated</t>
-  </si>
-  <si>
-    <t>NOTE: The Qs in column A that are red are the six questions that relate to societal impact.</t>
-  </si>
-  <si>
     <t>NOTE: N's were reverse coded</t>
   </si>
   <si>
@@ -516,7 +510,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,12 +520,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7E79"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,7 +550,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -585,28 +572,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -627,6 +605,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -947,11 +965,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0306057C-2408-A84E-8BC5-C7D6D6F6716B}">
   <dimension ref="A1:CN33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="17" topLeftCell="CJ18" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="5" ySplit="17" topLeftCell="CK18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="CK32" sqref="CK32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -966,10 +984,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:92" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="15"/>
       <c r="B1" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -1235,7 +1254,7 @@
       </c>
     </row>
     <row r="2" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1510,7 +1529,7 @@
       </c>
     </row>
     <row r="3" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1785,7 +1804,7 @@
       </c>
     </row>
     <row r="4" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -2060,7 +2079,7 @@
       </c>
     </row>
     <row r="5" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -2332,7 +2351,7 @@
       </c>
     </row>
     <row r="6" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -2604,7 +2623,7 @@
       </c>
     </row>
     <row r="7" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -2870,7 +2889,7 @@
       </c>
     </row>
     <row r="8" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -3145,7 +3164,7 @@
       </c>
     </row>
     <row r="9" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -3417,7 +3436,7 @@
       </c>
     </row>
     <row r="10" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -3692,7 +3711,7 @@
       </c>
     </row>
     <row r="11" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -3967,7 +3986,7 @@
       </c>
     </row>
     <row r="12" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -4242,7 +4261,7 @@
       </c>
     </row>
     <row r="13" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -4514,7 +4533,7 @@
       </c>
     </row>
     <row r="14" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -4789,7 +4808,7 @@
       </c>
     </row>
     <row r="15" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -5061,7 +5080,7 @@
       </c>
     </row>
     <row r="16" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -5334,7 +5353,7 @@
       </c>
     </row>
     <row r="17" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -5605,7 +5624,7 @@
       </c>
     </row>
     <row r="18" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -5878,7 +5897,7 @@
       </c>
     </row>
     <row r="19" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -6153,7 +6172,7 @@
       </c>
     </row>
     <row r="20" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -6428,7 +6447,7 @@
       </c>
     </row>
     <row r="21" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -6701,7 +6720,7 @@
       </c>
     </row>
     <row r="22" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -6973,7 +6992,7 @@
       </c>
     </row>
     <row r="23" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -7246,7 +7265,7 @@
       </c>
     </row>
     <row r="24" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -7514,350 +7533,351 @@
       </c>
     </row>
     <row r="25" spans="1:92" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
       <c r="CK25" s="2"/>
       <c r="CL25" s="2"/>
     </row>
-    <row r="26" spans="1:92" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="C26" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11" t="s">
+    <row r="26" spans="1:92" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="C26" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="8">
         <f>SUM(F2:F24)</f>
         <v>60</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="8">
         <f t="shared" ref="G26:BR26" si="3">SUM(G2:G24)</f>
         <v>60</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="8">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="8">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="8">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="8">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="8">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="M26" s="9">
+      <c r="M26" s="8">
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
-      <c r="N26" s="9">
+      <c r="N26" s="8">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="O26" s="9">
+      <c r="O26" s="8">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="P26" s="9">
+      <c r="P26" s="8">
         <f t="shared" si="3"/>
         <v>63</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="Q26" s="8">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="R26" s="9">
+      <c r="R26" s="8">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
-      <c r="S26" s="9">
+      <c r="S26" s="8">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
-      <c r="T26" s="9">
+      <c r="T26" s="8">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="U26" s="9">
+      <c r="U26" s="8">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="V26" s="9">
+      <c r="V26" s="8">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
-      <c r="W26" s="9">
+      <c r="W26" s="8">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
-      <c r="X26" s="9">
+      <c r="X26" s="8">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="Y26" s="9">
+      <c r="Y26" s="8">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
-      <c r="Z26" s="9">
+      <c r="Z26" s="8">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="AA26" s="9">
+      <c r="AA26" s="8">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="AB26" s="9">
+      <c r="AB26" s="8">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="AC26" s="9">
+      <c r="AC26" s="8">
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
-      <c r="AD26" s="9">
+      <c r="AD26" s="8">
         <f t="shared" si="3"/>
         <v>63</v>
       </c>
-      <c r="AE26" s="9">
+      <c r="AE26" s="8">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="AF26" s="9">
+      <c r="AF26" s="8">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
-      <c r="AG26" s="9">
+      <c r="AG26" s="8">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="AH26" s="9">
+      <c r="AH26" s="8">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="AI26" s="9">
+      <c r="AI26" s="8">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
-      <c r="AJ26" s="9">
+      <c r="AJ26" s="8">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="AK26" s="9">
+      <c r="AK26" s="8">
         <f t="shared" si="3"/>
         <v>63</v>
       </c>
-      <c r="AL26" s="9">
+      <c r="AL26" s="8">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
-      <c r="AM26" s="9">
+      <c r="AM26" s="8">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="AN26" s="9">
+      <c r="AN26" s="8">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="AO26" s="9">
+      <c r="AO26" s="8">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="AP26" s="9">
+      <c r="AP26" s="8">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="AQ26" s="9">
+      <c r="AQ26" s="8">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="AR26" s="9">
+      <c r="AR26" s="8">
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="AS26" s="9">
+      <c r="AS26" s="8">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="AT26" s="9">
+      <c r="AT26" s="8">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="AU26" s="9">
+      <c r="AU26" s="8">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="AV26" s="9">
+      <c r="AV26" s="8">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="AW26" s="9">
+      <c r="AW26" s="8">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
-      <c r="AX26" s="9">
+      <c r="AX26" s="8">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="AY26" s="9">
+      <c r="AY26" s="8">
         <f t="shared" si="3"/>
         <v>63</v>
       </c>
-      <c r="AZ26" s="9">
+      <c r="AZ26" s="8">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="BA26" s="9">
+      <c r="BA26" s="8">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="BB26" s="9">
+      <c r="BB26" s="8">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
-      <c r="BC26" s="9">
+      <c r="BC26" s="8">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
-      <c r="BD26" s="9">
+      <c r="BD26" s="8">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
-      <c r="BE26" s="9">
+      <c r="BE26" s="8">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
-      <c r="BF26" s="9">
+      <c r="BF26" s="8">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="BG26" s="9">
+      <c r="BG26" s="8">
         <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="BH26" s="9">
+      <c r="BH26" s="8">
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
-      <c r="BI26" s="9">
+      <c r="BI26" s="8">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
-      <c r="BJ26" s="9">
+      <c r="BJ26" s="8">
         <f t="shared" si="3"/>
         <v>73</v>
       </c>
-      <c r="BK26" s="9">
+      <c r="BK26" s="8">
         <f t="shared" si="3"/>
         <v>69</v>
       </c>
-      <c r="BL26" s="9">
+      <c r="BL26" s="8">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="BM26" s="9">
+      <c r="BM26" s="8">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
-      <c r="BN26" s="9">
+      <c r="BN26" s="8">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
-      <c r="BO26" s="9">
+      <c r="BO26" s="8">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="BP26" s="9">
+      <c r="BP26" s="8">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="BQ26" s="9">
+      <c r="BQ26" s="8">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="BR26" s="9">
+      <c r="BR26" s="8">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
-      <c r="BS26" s="9">
+      <c r="BS26" s="8">
         <f t="shared" ref="BS26:CI26" si="4">SUM(BS2:BS24)</f>
         <v>51</v>
       </c>
-      <c r="BT26" s="9">
+      <c r="BT26" s="8">
         <f t="shared" si="4"/>
         <v>49</v>
       </c>
-      <c r="BU26" s="9">
+      <c r="BU26" s="8">
         <f t="shared" si="4"/>
         <v>73</v>
       </c>
-      <c r="BV26" s="9">
+      <c r="BV26" s="8">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="BW26" s="9">
+      <c r="BW26" s="8">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="BX26" s="9">
+      <c r="BX26" s="8">
         <f t="shared" si="4"/>
         <v>58</v>
       </c>
-      <c r="BY26" s="9">
+      <c r="BY26" s="8">
         <f t="shared" si="4"/>
         <v>58</v>
       </c>
-      <c r="BZ26" s="9">
+      <c r="BZ26" s="8">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="CA26" s="9">
+      <c r="CA26" s="8">
         <f t="shared" si="4"/>
         <v>57</v>
       </c>
-      <c r="CB26" s="9">
+      <c r="CB26" s="8">
         <f t="shared" si="4"/>
         <v>61</v>
       </c>
-      <c r="CC26" s="9">
+      <c r="CC26" s="8">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="CD26" s="9">
+      <c r="CD26" s="8">
         <f t="shared" si="4"/>
         <v>55</v>
       </c>
-      <c r="CE26" s="9">
+      <c r="CE26" s="8">
         <f t="shared" si="4"/>
         <v>53</v>
       </c>
-      <c r="CF26" s="9">
+      <c r="CF26" s="8">
         <f t="shared" si="4"/>
         <v>61</v>
       </c>
-      <c r="CG26" s="9">
+      <c r="CG26" s="8">
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="CH26" s="9">
+      <c r="CH26" s="8">
         <f t="shared" si="4"/>
         <v>62</v>
       </c>
-      <c r="CI26" s="9">
+      <c r="CI26" s="8">
         <f t="shared" si="4"/>
         <v>64</v>
       </c>
-      <c r="CK26" s="12">
+      <c r="CK26" s="11">
         <f t="shared" ref="CK26" si="5">AVERAGE(F26:CI26)</f>
         <v>61.121951219512198</v>
       </c>
-      <c r="CL26" s="9" t="s">
+      <c r="CL26" s="8" t="s">
         <v>137</v>
       </c>
     </row>
@@ -7870,24 +7890,16 @@
         <v>138</v>
       </c>
       <c r="CN27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>144</v>
-      </c>
       <c r="CK28" s="2">
         <f>AVERAGE(CK2:CK24)</f>
         <v>2.68080058779399</v>
       </c>
       <c r="CL28" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:92" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:92" x14ac:dyDescent="0.2">
@@ -7908,23 +7920,31 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="89:90" x14ac:dyDescent="0.2">
+    <row r="33" spans="89:91" x14ac:dyDescent="0.2">
       <c r="CK33" s="3">
         <v>3.3</v>
       </c>
-      <c r="CL33" t="s">
-        <v>148</v>
+      <c r="CL33" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="CM33" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:D24">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CK2:CK24">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>$CK$33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CL2:CL24">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+      <formula>$CL$33</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7936,7 +7956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2B84AA0-4981-A640-B6F7-93E85735DCAD}">
   <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
@@ -8016,7 +8036,7 @@
       <c r="W1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Y1" s="15"/>
+      <c r="Y1" s="14"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -13796,7 +13816,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:W83 Y1">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="6" priority="2">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13940,7 +13960,7 @@
       <c r="O2">
         <v>4</v>
       </c>
-      <c r="P2" s="14">
+      <c r="P2" s="13">
         <f>'Transposed Responses'!P2</f>
         <v>2</v>
       </c>
@@ -14023,7 +14043,7 @@
       <c r="O3">
         <v>4</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="13">
         <f>'Transposed Responses'!P3</f>
         <v>2</v>
       </c>
@@ -14106,7 +14126,7 @@
       <c r="O4">
         <v>4</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="13">
         <f>'Transposed Responses'!P4</f>
         <v>2</v>
       </c>
@@ -14189,7 +14209,7 @@
       <c r="O5">
         <v>4</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="13">
         <f>'Transposed Responses'!P5</f>
         <v>2</v>
       </c>
@@ -14268,7 +14288,7 @@
       <c r="O6">
         <v>3</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="13">
         <f>'Transposed Responses'!P6</f>
         <v>3</v>
       </c>
@@ -14347,7 +14367,7 @@
       <c r="O7">
         <v>3</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="13">
         <f>'Transposed Responses'!P7</f>
         <v>3</v>
       </c>
@@ -14430,7 +14450,7 @@
       <c r="O8">
         <v>4</v>
       </c>
-      <c r="P8" s="14">
+      <c r="P8" s="13">
         <f>'Transposed Responses'!P8</f>
         <v>2</v>
       </c>
@@ -14513,7 +14533,7 @@
       <c r="O9">
         <v>4</v>
       </c>
-      <c r="P9" s="14">
+      <c r="P9" s="13">
         <f>'Transposed Responses'!P9</f>
         <v>3</v>
       </c>
@@ -14585,7 +14605,7 @@
       <c r="O10">
         <v>3</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="13">
         <f>'Transposed Responses'!P10</f>
         <v>3</v>
       </c>
@@ -14668,7 +14688,7 @@
       <c r="O11">
         <v>4</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="13">
         <f>'Transposed Responses'!P11</f>
         <v>2</v>
       </c>
@@ -14751,7 +14771,7 @@
       <c r="O12">
         <v>4</v>
       </c>
-      <c r="P12" s="14">
+      <c r="P12" s="13">
         <f>'Transposed Responses'!P12</f>
         <v>2</v>
       </c>
@@ -14834,7 +14854,7 @@
       <c r="O13">
         <v>3</v>
       </c>
-      <c r="P13" s="14">
+      <c r="P13" s="13">
         <f>'Transposed Responses'!P13</f>
         <v>3</v>
       </c>
@@ -14917,7 +14937,7 @@
       <c r="O14">
         <v>4</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="13">
         <f>'Transposed Responses'!P14</f>
         <v>2</v>
       </c>
@@ -15000,7 +15020,7 @@
       <c r="O15">
         <v>3</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="13">
         <f>'Transposed Responses'!P15</f>
         <v>2</v>
       </c>
@@ -15076,7 +15096,7 @@
       <c r="O16">
         <v>3</v>
       </c>
-      <c r="P16" s="14">
+      <c r="P16" s="13">
         <f>'Transposed Responses'!P16</f>
         <v>2</v>
       </c>
@@ -15156,7 +15176,7 @@
       <c r="O17">
         <v>4</v>
       </c>
-      <c r="P17" s="14">
+      <c r="P17" s="13">
         <f>'Transposed Responses'!P17</f>
         <v>2</v>
       </c>
@@ -15239,7 +15259,7 @@
       <c r="O18">
         <v>3</v>
       </c>
-      <c r="P18" s="14">
+      <c r="P18" s="13">
         <f>'Transposed Responses'!P18</f>
         <v>3</v>
       </c>
@@ -15322,7 +15342,7 @@
       <c r="O19">
         <v>3</v>
       </c>
-      <c r="P19" s="14">
+      <c r="P19" s="13">
         <f>'Transposed Responses'!P19</f>
         <v>1</v>
       </c>
@@ -15405,7 +15425,7 @@
       <c r="O20">
         <v>2</v>
       </c>
-      <c r="P20" s="14">
+      <c r="P20" s="13">
         <f>'Transposed Responses'!P20</f>
         <v>1</v>
       </c>
@@ -15488,7 +15508,7 @@
       <c r="O21">
         <v>3</v>
       </c>
-      <c r="P21" s="14">
+      <c r="P21" s="13">
         <f>'Transposed Responses'!P21</f>
         <v>1</v>
       </c>
@@ -15571,7 +15591,7 @@
       <c r="O22">
         <v>4</v>
       </c>
-      <c r="P22" s="14">
+      <c r="P22" s="13">
         <f>'Transposed Responses'!P22</f>
         <v>3</v>
       </c>
@@ -15654,7 +15674,7 @@
       <c r="O23">
         <v>4</v>
       </c>
-      <c r="P23" s="14">
+      <c r="P23" s="13">
         <f>'Transposed Responses'!P23</f>
         <v>3</v>
       </c>
@@ -15737,7 +15757,7 @@
       <c r="O24">
         <v>4</v>
       </c>
-      <c r="P24" s="14">
+      <c r="P24" s="13">
         <f>'Transposed Responses'!P24</f>
         <v>3</v>
       </c>
@@ -15820,7 +15840,7 @@
       <c r="O25">
         <v>3</v>
       </c>
-      <c r="P25" s="14">
+      <c r="P25" s="13">
         <f>'Transposed Responses'!P25</f>
         <v>3</v>
       </c>
@@ -15903,7 +15923,7 @@
       <c r="O26">
         <v>3</v>
       </c>
-      <c r="P26" s="14">
+      <c r="P26" s="13">
         <f>'Transposed Responses'!P26</f>
         <v>2</v>
       </c>
@@ -15986,7 +16006,7 @@
       <c r="O27">
         <v>3</v>
       </c>
-      <c r="P27" s="14">
+      <c r="P27" s="13">
         <f>'Transposed Responses'!P27</f>
         <v>3</v>
       </c>
@@ -16069,7 +16089,7 @@
       <c r="O28">
         <v>4</v>
       </c>
-      <c r="P28" s="14">
+      <c r="P28" s="13">
         <f>'Transposed Responses'!P28</f>
         <v>3</v>
       </c>
@@ -16152,7 +16172,7 @@
       <c r="O29">
         <v>2</v>
       </c>
-      <c r="P29" s="14">
+      <c r="P29" s="13">
         <f>'Transposed Responses'!P29</f>
         <v>2</v>
       </c>
@@ -16235,7 +16255,7 @@
       <c r="O30">
         <v>3</v>
       </c>
-      <c r="P30" s="14">
+      <c r="P30" s="13">
         <f>'Transposed Responses'!P30</f>
         <v>3</v>
       </c>
@@ -16318,7 +16338,7 @@
       <c r="O31">
         <v>3</v>
       </c>
-      <c r="P31" s="14">
+      <c r="P31" s="13">
         <f>'Transposed Responses'!P31</f>
         <v>1</v>
       </c>
@@ -16401,7 +16421,7 @@
       <c r="O32">
         <v>4</v>
       </c>
-      <c r="P32" s="14">
+      <c r="P32" s="13">
         <f>'Transposed Responses'!P32</f>
         <v>4</v>
       </c>
@@ -16480,7 +16500,7 @@
       <c r="O33">
         <v>4</v>
       </c>
-      <c r="P33" s="14">
+      <c r="P33" s="13">
         <f>'Transposed Responses'!P33</f>
         <v>2</v>
       </c>
@@ -16563,7 +16583,7 @@
       <c r="O34">
         <v>3</v>
       </c>
-      <c r="P34" s="14">
+      <c r="P34" s="13">
         <f>'Transposed Responses'!P34</f>
         <v>2</v>
       </c>
@@ -16646,7 +16666,7 @@
       <c r="O35">
         <v>4</v>
       </c>
-      <c r="P35" s="14">
+      <c r="P35" s="13">
         <f>'Transposed Responses'!P35</f>
         <v>3</v>
       </c>
@@ -16729,7 +16749,7 @@
       <c r="O36">
         <v>4</v>
       </c>
-      <c r="P36" s="14">
+      <c r="P36" s="13">
         <f>'Transposed Responses'!P36</f>
         <v>3</v>
       </c>
@@ -16812,7 +16832,7 @@
       <c r="O37">
         <v>3</v>
       </c>
-      <c r="P37" s="14">
+      <c r="P37" s="13">
         <f>'Transposed Responses'!P37</f>
         <v>3</v>
       </c>
@@ -16895,7 +16915,7 @@
       <c r="O38">
         <v>4</v>
       </c>
-      <c r="P38" s="14">
+      <c r="P38" s="13">
         <f>'Transposed Responses'!P38</f>
         <v>2</v>
       </c>
@@ -16978,7 +16998,7 @@
       <c r="O39">
         <v>3</v>
       </c>
-      <c r="P39" s="14">
+      <c r="P39" s="13">
         <f>'Transposed Responses'!P39</f>
         <v>3</v>
       </c>
@@ -17061,7 +17081,7 @@
       <c r="O40">
         <v>4</v>
       </c>
-      <c r="P40" s="14">
+      <c r="P40" s="13">
         <f>'Transposed Responses'!P40</f>
         <v>3</v>
       </c>
@@ -17144,7 +17164,7 @@
       <c r="O41">
         <v>4</v>
       </c>
-      <c r="P41" s="14">
+      <c r="P41" s="13">
         <f>'Transposed Responses'!P41</f>
         <v>1</v>
       </c>
@@ -17227,7 +17247,7 @@
       <c r="O42">
         <v>4</v>
       </c>
-      <c r="P42" s="14">
+      <c r="P42" s="13">
         <f>'Transposed Responses'!P42</f>
         <v>3</v>
       </c>
@@ -17310,7 +17330,7 @@
       <c r="O43">
         <v>4</v>
       </c>
-      <c r="P43" s="14">
+      <c r="P43" s="13">
         <f>'Transposed Responses'!P43</f>
         <v>1</v>
       </c>
@@ -17393,7 +17413,7 @@
       <c r="O44">
         <v>4</v>
       </c>
-      <c r="P44" s="14">
+      <c r="P44" s="13">
         <f>'Transposed Responses'!P44</f>
         <v>1</v>
       </c>
@@ -17476,7 +17496,7 @@
       <c r="O45">
         <v>3</v>
       </c>
-      <c r="P45" s="14">
+      <c r="P45" s="13">
         <f>'Transposed Responses'!P45</f>
         <v>1</v>
       </c>
@@ -17559,7 +17579,7 @@
       <c r="O46">
         <v>3</v>
       </c>
-      <c r="P46" s="14">
+      <c r="P46" s="13">
         <f>'Transposed Responses'!P46</f>
         <v>3</v>
       </c>
@@ -17638,7 +17658,7 @@
       <c r="O47">
         <v>3</v>
       </c>
-      <c r="P47" s="14">
+      <c r="P47" s="13">
         <f>'Transposed Responses'!P47</f>
         <v>3</v>
       </c>
@@ -17721,7 +17741,7 @@
       <c r="O48">
         <v>4</v>
       </c>
-      <c r="P48" s="14">
+      <c r="P48" s="13">
         <f>'Transposed Responses'!P48</f>
         <v>3</v>
       </c>
@@ -17804,7 +17824,7 @@
       <c r="O49">
         <v>4</v>
       </c>
-      <c r="P49" s="14">
+      <c r="P49" s="13">
         <f>'Transposed Responses'!P49</f>
         <v>1</v>
       </c>
@@ -17887,7 +17907,7 @@
       <c r="O50">
         <v>3</v>
       </c>
-      <c r="P50" s="14">
+      <c r="P50" s="13">
         <f>'Transposed Responses'!P50</f>
         <v>2</v>
       </c>
@@ -17970,7 +17990,7 @@
       <c r="O51" s="1">
         <v>3</v>
       </c>
-      <c r="P51" s="14"/>
+      <c r="P51" s="13"/>
       <c r="Q51">
         <f>5-'Transposed Responses'!Q51</f>
         <v>2</v>
@@ -18050,7 +18070,7 @@
       <c r="O52" s="1">
         <v>4</v>
       </c>
-      <c r="P52" s="14">
+      <c r="P52" s="13">
         <f>'Transposed Responses'!P52</f>
         <v>3</v>
       </c>
@@ -18133,7 +18153,7 @@
       <c r="O53" s="1">
         <v>4</v>
       </c>
-      <c r="P53" s="14">
+      <c r="P53" s="13">
         <f>'Transposed Responses'!P53</f>
         <v>3</v>
       </c>
@@ -18216,7 +18236,7 @@
       <c r="O54" s="1">
         <v>4</v>
       </c>
-      <c r="P54" s="14">
+      <c r="P54" s="13">
         <f>'Transposed Responses'!P54</f>
         <v>3</v>
       </c>
@@ -18299,7 +18319,7 @@
       <c r="O55" s="1">
         <v>4</v>
       </c>
-      <c r="P55" s="14">
+      <c r="P55" s="13">
         <f>'Transposed Responses'!P55</f>
         <v>2</v>
       </c>
@@ -18382,7 +18402,7 @@
       <c r="O56" s="1">
         <v>4</v>
       </c>
-      <c r="P56" s="14">
+      <c r="P56" s="13">
         <f>'Transposed Responses'!P56</f>
         <v>2</v>
       </c>
@@ -18465,7 +18485,7 @@
       <c r="O57" s="1">
         <v>2</v>
       </c>
-      <c r="P57" s="14">
+      <c r="P57" s="13">
         <f>'Transposed Responses'!P57</f>
         <v>1</v>
       </c>
@@ -18548,7 +18568,7 @@
       <c r="O58" s="1">
         <v>4</v>
       </c>
-      <c r="P58" s="14">
+      <c r="P58" s="13">
         <f>'Transposed Responses'!P58</f>
         <v>3</v>
       </c>
@@ -18627,7 +18647,7 @@
       <c r="O59" s="1">
         <v>4</v>
       </c>
-      <c r="P59" s="14">
+      <c r="P59" s="13">
         <f>'Transposed Responses'!P59</f>
         <v>3</v>
       </c>
@@ -18710,7 +18730,7 @@
       <c r="O60" s="1">
         <v>3</v>
       </c>
-      <c r="P60" s="14">
+      <c r="P60" s="13">
         <f>'Transposed Responses'!P60</f>
         <v>3</v>
       </c>
@@ -18793,7 +18813,7 @@
       <c r="O61" s="1">
         <v>3</v>
       </c>
-      <c r="P61" s="14">
+      <c r="P61" s="13">
         <f>'Transposed Responses'!P61</f>
         <v>3</v>
       </c>
@@ -18872,7 +18892,7 @@
       <c r="O62" s="1">
         <v>2</v>
       </c>
-      <c r="P62" s="14">
+      <c r="P62" s="13">
         <f>'Transposed Responses'!P62</f>
         <v>1</v>
       </c>
@@ -18955,7 +18975,7 @@
       <c r="O63" s="1">
         <v>2</v>
       </c>
-      <c r="P63" s="14">
+      <c r="P63" s="13">
         <f>'Transposed Responses'!P63</f>
         <v>3</v>
       </c>
@@ -19038,7 +19058,7 @@
       <c r="O64" s="1">
         <v>3</v>
       </c>
-      <c r="P64" s="14">
+      <c r="P64" s="13">
         <f>'Transposed Responses'!P64</f>
         <v>3</v>
       </c>
@@ -19121,7 +19141,7 @@
       <c r="O65" s="1">
         <v>3</v>
       </c>
-      <c r="P65" s="14">
+      <c r="P65" s="13">
         <f>'Transposed Responses'!P65</f>
         <v>3</v>
       </c>
@@ -19204,7 +19224,7 @@
       <c r="O66" s="1">
         <v>3</v>
       </c>
-      <c r="P66" s="14">
+      <c r="P66" s="13">
         <f>'Transposed Responses'!P66</f>
         <v>3</v>
       </c>
@@ -19287,7 +19307,7 @@
       <c r="O67" s="1">
         <v>2</v>
       </c>
-      <c r="P67" s="14">
+      <c r="P67" s="13">
         <f>'Transposed Responses'!P67</f>
         <v>1</v>
       </c>
@@ -19370,7 +19390,7 @@
       <c r="O68" s="1">
         <v>3</v>
       </c>
-      <c r="P68" s="14">
+      <c r="P68" s="13">
         <f>'Transposed Responses'!P68</f>
         <v>1</v>
       </c>
@@ -19453,7 +19473,7 @@
       <c r="O69" s="1">
         <v>3</v>
       </c>
-      <c r="P69" s="14">
+      <c r="P69" s="13">
         <f>'Transposed Responses'!P69</f>
         <v>3</v>
       </c>
@@ -19534,7 +19554,7 @@
         <v>2</v>
       </c>
       <c r="O70" s="1"/>
-      <c r="P70" s="14"/>
+      <c r="P70" s="13"/>
       <c r="R70">
         <f>'Transposed Responses'!R70</f>
         <v>3</v>
@@ -19604,7 +19624,7 @@
       <c r="O71" s="1">
         <v>4</v>
       </c>
-      <c r="P71" s="14">
+      <c r="P71" s="13">
         <f>'Transposed Responses'!P71</f>
         <v>2</v>
       </c>
@@ -19687,7 +19707,7 @@
       <c r="O72" s="1">
         <v>3</v>
       </c>
-      <c r="P72" s="14">
+      <c r="P72" s="13">
         <f>'Transposed Responses'!P72</f>
         <v>3</v>
       </c>
@@ -19770,7 +19790,7 @@
       <c r="O73" s="1">
         <v>2</v>
       </c>
-      <c r="P73" s="14">
+      <c r="P73" s="13">
         <f>'Transposed Responses'!P73</f>
         <v>1</v>
       </c>
@@ -19853,7 +19873,7 @@
       <c r="O74" s="1">
         <v>3</v>
       </c>
-      <c r="P74" s="14">
+      <c r="P74" s="13">
         <f>'Transposed Responses'!P74</f>
         <v>2</v>
       </c>
@@ -19936,7 +19956,7 @@
       <c r="O75" s="1">
         <v>3</v>
       </c>
-      <c r="P75" s="14">
+      <c r="P75" s="13">
         <f>'Transposed Responses'!P75</f>
         <v>1</v>
       </c>
@@ -20019,7 +20039,7 @@
       <c r="O76" s="1">
         <v>3</v>
       </c>
-      <c r="P76" s="14">
+      <c r="P76" s="13">
         <f>'Transposed Responses'!P76</f>
         <v>2</v>
       </c>
@@ -20102,7 +20122,7 @@
       <c r="O77" s="1">
         <v>3</v>
       </c>
-      <c r="P77" s="14">
+      <c r="P77" s="13">
         <f>'Transposed Responses'!P77</f>
         <v>1</v>
       </c>
@@ -20185,7 +20205,7 @@
       <c r="O78" s="1">
         <v>3</v>
       </c>
-      <c r="P78" s="14">
+      <c r="P78" s="13">
         <f>'Transposed Responses'!P78</f>
         <v>2</v>
       </c>
@@ -20268,7 +20288,7 @@
       <c r="O79" s="1">
         <v>3</v>
       </c>
-      <c r="P79" s="14">
+      <c r="P79" s="13">
         <f>'Transposed Responses'!P79</f>
         <v>2</v>
       </c>
@@ -20351,7 +20371,7 @@
       <c r="O80" s="1">
         <v>4</v>
       </c>
-      <c r="P80" s="14">
+      <c r="P80" s="13">
         <f>'Transposed Responses'!P80</f>
         <v>2</v>
       </c>
@@ -20434,7 +20454,7 @@
       <c r="O81" s="1">
         <v>3</v>
       </c>
-      <c r="P81" s="14">
+      <c r="P81" s="13">
         <f>'Transposed Responses'!P81</f>
         <v>2</v>
       </c>
@@ -20517,7 +20537,7 @@
       <c r="O82" s="1">
         <v>3</v>
       </c>
-      <c r="P82" s="14">
+      <c r="P82" s="13">
         <f>'Transposed Responses'!P82</f>
         <v>2</v>
       </c>
@@ -20600,7 +20620,7 @@
       <c r="O83" s="1">
         <v>3</v>
       </c>
-      <c r="P83" s="14">
+      <c r="P83" s="13">
         <f>'Transposed Responses'!P83</f>
         <v>4</v>
       </c>
@@ -20633,7 +20653,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:W83">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>